<commit_message>
Fixed premake5.lua with EOP_DISABLE_LOGGING
</commit_message>
<xml_diff>
--- a/examples/seating_plan/spreadsheets/example-classroom_seating_plan-org.xlsx
+++ b/examples/seating_plan/spreadsheets/example-classroom_seating_plan-org.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\cpp\entity_organisation_program\examples\seating_plan\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2FC7C6-96A0-4765-A31A-405884845250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCBE4D2-C6D9-45D4-891F-0C503E5B81FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>Organised Seating Plan</t>
   </si>
@@ -123,6 +123,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts>
+	</numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -506,34 +508,34 @@
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -541,31 +543,31 @@
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -573,25 +575,25 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Updated README.md and Documentation
</commit_message>
<xml_diff>
--- a/examples/seating_plan/spreadsheets/example-classroom_seating_plan-org.xlsx
+++ b/examples/seating_plan/spreadsheets/example-classroom_seating_plan-org.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\cpp\entity_organisation_program\examples\seating_plan\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCBE4D2-C6D9-45D4-891F-0C503E5B81FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A5240A-25FC-43C9-8C6E-6F3C6AD89DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Organised Seating Plan</t>
   </si>
@@ -123,8 +123,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts>
-	</numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -508,34 +506,34 @@
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -543,16 +541,16 @@
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>26</v>
@@ -561,13 +559,13 @@
         <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -575,25 +573,25 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>

</xml_diff>